<commit_message>
rearrange exps, and spanish version
</commit_message>
<xml_diff>
--- a/exp/empathy_intonation_perc/instructions/lextale_instructions_text.xlsx
+++ b/exp/empathy_intonation_perc/instructions/lextale_instructions_text.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -361,52 +361,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Este es un test de vocabulario en español. 
-  A continuación vas a ver 90 secuencias de letras que parecen 'españolas'.
-  Solo algunas de ellas son palabras de verdad.</t>
+          <t>Great! Now we will move on. The next task consists of about 60 trials, in each of which you will see a string of letters. 
+  Your task is to decide whether this is a real Spanish word or not.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(presiona la barra espaciadora para continuar)</t>
+          <t>(press the spacebar to continue)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Por favor, señala las palabras que tú conoces (aquellas que estás convencido que son palabras españolas, incluso aunque no seas capaz de dar el significado preciso).</t>
+          <t>If you think it is an existing Spanish word, you type '1' (for 'REAL'), and if you think it is not an existing Spanish word, you type '0' (for 'FAKE').</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(presiona la barra espaciadora para continuar)</t>
+          <t>(press the spacebar to continue)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pero cuidado: los errores se penalizan. Por eso no tiene sentido tratar de incrementar tu puntuación marcando como reales palabras que nunca has visto.</t>
+          <t>If you are sure that the word exists, even though you don’t know its exact meaning, you may still respond '1' (REAL). 
+  But if you are not sure if it is an existing word, you should respond '0' (FAKE).
+  Let's do a practice round...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(presiona la barra espaciadora para continuar)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Presiona la tecla 1 si piensas que es una palabra real y la tecla 
-  0 si piensas que es una palabra falsa. 
-  Vamos a practicar un poco...</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(presiona la barra espaciadora para continuar)</t>
+          <t>(press the spacebar to continue)</t>
         </is>
       </c>
     </row>

</xml_diff>